<commit_message>
Added Testing Phase for the processed Test Split
</commit_message>
<xml_diff>
--- a/Results_12W/Disease_Specific_Analysis/tables/Table2_Model_Performance_by_Disease_Group.xlsx
+++ b/Results_12W/Disease_Specific_Analysis/tables/Table2_Model_Performance_by_Disease_Group.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Disease_Group</t>
   </si>
@@ -26,15 +39,6 @@
   </si>
   <si>
     <t>MAE</t>
-  </si>
-  <si>
-    <t>MSE</t>
-  </si>
-  <si>
-    <t>RMSE</t>
-  </si>
-  <si>
-    <t>Mean_Absolute_Error</t>
   </si>
   <si>
     <t>Mean_Prediction</t>
@@ -67,13 +71,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -81,19 +91,356 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -116,9 +463,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -126,11 +715,63 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -413,19 +1054,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,19 +1096,10 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>12</v>
       </c>
       <c r="B2">
         <v>108</v>
@@ -477,71 +1111,53 @@
         <v>1.551</v>
       </c>
       <c r="E2">
-        <v>4.188</v>
+        <v>8.42</v>
       </c>
       <c r="F2">
-        <v>2.046</v>
+        <v>8.51</v>
       </c>
       <c r="G2">
-        <v>1.551</v>
+        <v>6.46</v>
       </c>
       <c r="H2">
-        <v>8.42</v>
+        <v>7.65</v>
       </c>
       <c r="I2">
-        <v>8.51</v>
-      </c>
-      <c r="J2">
-        <v>6.46</v>
-      </c>
-      <c r="K2">
-        <v>7.65</v>
-      </c>
-      <c r="L2">
         <v>0.972</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>39</v>
       </c>
       <c r="C3">
-        <v>0.8120000000000001</v>
+        <v>0.812</v>
       </c>
       <c r="D3">
         <v>1.646</v>
       </c>
       <c r="E3">
-        <v>4.799</v>
+        <v>5.72</v>
       </c>
       <c r="F3">
-        <v>2.191</v>
+        <v>5.38</v>
       </c>
       <c r="G3">
-        <v>1.646</v>
+        <v>3.51</v>
       </c>
       <c r="H3">
-        <v>5.72</v>
+        <v>5.05</v>
       </c>
       <c r="I3">
-        <v>5.38</v>
-      </c>
-      <c r="J3">
-        <v>3.51</v>
-      </c>
-      <c r="K3">
-        <v>5.05</v>
-      </c>
-      <c r="L3">
-        <v>0.9340000000000001</v>
+        <v>0.934</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -553,33 +1169,24 @@
         <v>1.199</v>
       </c>
       <c r="E4">
-        <v>2.631</v>
+        <v>3.86</v>
       </c>
       <c r="F4">
-        <v>1.622</v>
+        <v>3.5</v>
       </c>
       <c r="G4">
-        <v>1.199</v>
+        <v>4.49</v>
       </c>
       <c r="H4">
-        <v>3.86</v>
+        <v>5.82</v>
       </c>
       <c r="I4">
-        <v>3.5</v>
-      </c>
-      <c r="J4">
-        <v>4.49</v>
-      </c>
-      <c r="K4">
-        <v>5.82</v>
-      </c>
-      <c r="L4">
         <v>0.986</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -591,31 +1198,23 @@
         <v>2.434</v>
       </c>
       <c r="E5">
-        <v>7.555</v>
+        <v>8.31</v>
       </c>
       <c r="F5">
-        <v>2.749</v>
+        <v>8.5</v>
       </c>
       <c r="G5">
-        <v>2.434</v>
+        <v>6.82</v>
       </c>
       <c r="H5">
-        <v>8.31</v>
+        <v>8.22</v>
       </c>
       <c r="I5">
-        <v>8.5</v>
-      </c>
-      <c r="J5">
-        <v>6.82</v>
-      </c>
-      <c r="K5">
-        <v>8.220000000000001</v>
-      </c>
-      <c r="L5">
         <v>0.951</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>